<commit_message>
feat: add the waiting minutes
</commit_message>
<xml_diff>
--- a/post-management-sheets-template.xlsx
+++ b/post-management-sheets-template.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamiya/github.com/ryohei-kamiya/pushy-reminder/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE3CDC-2387-EC4A-A88B-C6CEBA1B07B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="main" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="holiday_calendars" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="completion_keywords" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="settings" sheetId="4" r:id="rId7"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="holiday_calendars" sheetId="2" r:id="rId2"/>
+    <sheet name="completion_keywords" sheetId="3" r:id="rId3"/>
+    <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>No.</t>
   </si>
@@ -43,9 +52,6 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Remind message</t>
-  </si>
-  <si>
     <t>Not remind to</t>
   </si>
   <si>
@@ -61,12 +67,6 @@
     <t>channel</t>
   </si>
   <si>
-    <t>This is a request message of a task.</t>
-  </si>
-  <si>
-    <t>If you have done it, please let us know "done" in the thread.</t>
-  </si>
-  <si>
     <t>calendar id</t>
   </si>
   <si>
@@ -131,32 +131,61 @@
   </si>
   <si>
     <t>DEBUG</t>
+  </si>
+  <si>
+    <t>Reminder message</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Waiting minutes</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Today is the deadline for the monthly report.
+If you have already submitted, please post "Done" in this thread.</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Not done yet?</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -165,75 +194,58 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -423,31 +435,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.63"/>
-    <col customWidth="1" min="2" max="2" width="28.63"/>
-    <col customWidth="1" min="3" max="3" width="29.38"/>
-    <col customWidth="1" min="4" max="4" width="19.75"/>
-    <col customWidth="1" min="7" max="7" width="15.88"/>
-    <col customWidth="1" min="8" max="8" width="16.5"/>
-    <col customWidth="1" min="9" max="9" width="32.13"/>
-    <col customWidth="1" min="10" max="10" width="20.88"/>
-    <col customWidth="1" min="11" max="11" width="19.25"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="10" width="32.1640625" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,27 +493,30 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>1</v>
@@ -505,200 +525,210 @@
         <v>0.375</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="1" t="b">
+        <v>38</v>
+      </c>
+      <c r="J2" s="5">
+        <v>480</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="80.38"/>
+    <col min="1" max="1" width="80.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.75"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="29.75"/>
-    <col customWidth="1" min="2" max="2" width="16.88"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="B6" s="6">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="B8" s="6">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="7">
-        <v>1440.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="8">
-        <v>1440.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
+      <c r="B11" s="7">
+        <v>0.99998842592592596</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0.999988425925926</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="10" t="b">
+      <c r="B12" s="8" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: schedule by day of the week(#6)
</commit_message>
<xml_diff>
--- a/post-management-sheets-template.xlsx
+++ b/post-management-sheets-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamiya/github.com/ryohei-kamiya/pushy-reminder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE3CDC-2387-EC4A-A88B-C6CEBA1B07B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF9FD97-BA10-E74A-BCD8-49FD6E3E30F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>No.</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>BOT_NAME</t>
-  </si>
-  <si>
-    <t>PushyReminder</t>
   </si>
   <si>
     <t>ACTIVE_CHAT_APP</t>
@@ -147,6 +144,18 @@
   </si>
   <si>
     <t>Not done yet?</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>EndlessReminder</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CHATWORK_API_TOKEN</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Fri</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -445,10 +454,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -493,10 +502,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -531,15 +540,53 @@
         <v>13</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="5">
         <v>480</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="5">
+        <v>480</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -624,9 +671,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -647,83 +696,89 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1440</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="6">
-        <v>1</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6">
-        <v>1440</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="7">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7">
-        <v>0.99998842592592596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="8" t="b">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.99998842592592596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feat schedule by day of the week #6 (#7)
* feat: schedule by day of the week(#6)
</commit_message>
<xml_diff>
--- a/post-management-sheets-template.xlsx
+++ b/post-management-sheets-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamiya/github.com/ryohei-kamiya/pushy-reminder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE3CDC-2387-EC4A-A88B-C6CEBA1B07B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF9FD97-BA10-E74A-BCD8-49FD6E3E30F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>No.</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>BOT_NAME</t>
-  </si>
-  <si>
-    <t>PushyReminder</t>
   </si>
   <si>
     <t>ACTIVE_CHAT_APP</t>
@@ -147,6 +144,18 @@
   </si>
   <si>
     <t>Not done yet?</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>EndlessReminder</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CHATWORK_API_TOKEN</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Fri</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -445,10 +454,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -493,10 +502,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -531,15 +540,53 @@
         <v>13</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="5">
         <v>480</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="56" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="5">
+        <v>480</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -624,9 +671,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -647,83 +696,89 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1440</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="6">
-        <v>1</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6">
-        <v>1440</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="7">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7">
-        <v>0.99998842592592596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="8" t="b">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.99998842592592596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>